<commit_message>
Updated ER diagram and Sprint backlog
Updated ER diagram to included nullable AssignedGroupId column in Stage table

Updated sprint backlog by removing all task associated requirements
</commit_message>
<xml_diff>
--- a/Sprints/Sprint2/G4CapstoneProject_Sprint2_Backlog_Burndown.xlsx
+++ b/Sprints/Sprint2/G4CapstoneProject_Sprint2_Backlog_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Documents\GitHub\Capstone-Project\Sprints\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DC52232-7B8E-42A3-9FFE-0DDC0E1A9EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AAEB7D-706D-4EFA-801E-35AF863ACAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="2400" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>Related User Story</t>
   </si>
@@ -101,39 +101,12 @@
     <t>Implement base project board page</t>
   </si>
   <si>
-    <t>Manager - Assign a task on a board from a project for my group to an employee in my group</t>
-  </si>
-  <si>
-    <t>Implement view to assign task to an employee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement functionality/testing to assign an employee of your group to a task </t>
-  </si>
-  <si>
     <t>Admin - View and Edit a board for a project</t>
   </si>
   <si>
-    <t xml:space="preserve">Implement functionality/testing to assign an employee to a task </t>
-  </si>
-  <si>
-    <t>Admin - Assign a task on a board from a project to any employee that’s in a group assigned to that project</t>
-  </si>
-  <si>
     <t>Employee - View board</t>
   </si>
   <si>
-    <t>Employee - Create a task on the board of a project for my group</t>
-  </si>
-  <si>
-    <t>Implement view to create tasks</t>
-  </si>
-  <si>
-    <t>Employee - Update status of my assigned task</t>
-  </si>
-  <si>
-    <t>Implement view to update status</t>
-  </si>
-  <si>
     <t>Implement functionality/testing to delete stages</t>
   </si>
   <si>
@@ -143,60 +116,12 @@
     <t>Implement view to add stages</t>
   </si>
   <si>
-    <t>Implement functionality/testing to create tasks</t>
-  </si>
-  <si>
-    <t>Manager - Create a task on the board of a project for my group</t>
-  </si>
-  <si>
-    <t>Implement functionality/testing to delete tasks</t>
-  </si>
-  <si>
-    <t>Implement view to delete tasks</t>
-  </si>
-  <si>
-    <t>Implement functionality/testing to edit tasks</t>
-  </si>
-  <si>
-    <t>Implement view to edit tasks</t>
-  </si>
-  <si>
-    <t>Manager - Update status of  assigned task</t>
-  </si>
-  <si>
-    <t>Admin - Update status of any task</t>
-  </si>
-  <si>
-    <t>Admin - Create a task on the board of a project</t>
-  </si>
-  <si>
-    <t>Implement functionality/testing to update status of a task</t>
-  </si>
-  <si>
-    <t>Implement functionality/testing to update status of my assigned task</t>
-  </si>
-  <si>
-    <t>Implement functionality/testing to update status of your employees' assigned tasks</t>
-  </si>
-  <si>
     <t>Implement functionality/testing to edit stages</t>
   </si>
   <si>
     <t>Implement view to edit stages</t>
   </si>
   <si>
-    <t>Implement functionality/testing to delete tasks created by myself</t>
-  </si>
-  <si>
-    <t>Implement view to delete tasks created by myself</t>
-  </si>
-  <si>
-    <t>Implement functionality/testing to edit tasks created by myself</t>
-  </si>
-  <si>
-    <t>Implement view to edit tasks created by myself</t>
-  </si>
-  <si>
     <t>Users - Can change password if I forgot it</t>
   </si>
   <si>
@@ -206,12 +131,6 @@
     <t>Implement view to forgot password page</t>
   </si>
   <si>
-    <t>Users - I can look up username by email if I forgot username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement functionality/testing to look up username based on email </t>
-  </si>
-  <si>
     <t>Implement view to find username page</t>
   </si>
   <si>
@@ -261,6 +180,12 @@
   </si>
   <si>
     <t xml:space="preserve">system should display groups that have been requested to assign for a project, but have not approved yet	</t>
+  </si>
+  <si>
+    <t>Users - I can retrieve my username by email if I forgot username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement functionality/testing to send username using the email associated with it  </t>
   </si>
 </sst>
 </file>
@@ -481,7 +406,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$86:$E$86</c:f>
+              <c:f>Sheet1!$C$50:$E$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1534,10 +1459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,7 +1537,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
@@ -1621,7 +1546,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
@@ -1630,7 +1555,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
@@ -1639,7 +1564,7 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
@@ -1648,7 +1573,7 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
@@ -1661,12 +1586,12 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
@@ -1675,7 +1600,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
@@ -1683,17 +1608,17 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>36</v>
-      </c>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
@@ -1702,7 +1627,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
@@ -1711,7 +1636,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
@@ -1720,7 +1645,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
@@ -1728,17 +1653,17 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
@@ -1753,10 +1678,10 @@
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
@@ -1765,7 +1690,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
@@ -1778,12 +1703,12 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
@@ -1792,7 +1717,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
@@ -1800,17 +1725,17 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
-      <c r="B27" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="B28" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
@@ -1819,25 +1744,25 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
-      <c r="B30" s="1" t="s">
-        <v>47</v>
+      <c r="B30" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="1" t="s">
-        <v>48</v>
+      <c r="B31" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
@@ -1845,17 +1770,17 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>26</v>
-      </c>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
       <c r="B33" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
@@ -1864,25 +1789,25 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
-      <c r="B35" s="1"/>
+      <c r="B35" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>43</v>
-      </c>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1891,7 +1816,7 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1900,7 +1825,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1909,7 +1834,7 @@
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -1918,7 +1843,7 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
@@ -1927,446 +1852,132 @@
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="1"/>
+      <c r="B42" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>44</v>
-      </c>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
-      <c r="B44" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="A45" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="A46" s="6"/>
       <c r="B46" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>28</v>
-      </c>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
       <c r="B48" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-      <c r="B59" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="B62" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="B65" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-    </row>
-    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-    </row>
-    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C70" s="1"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C72" s="1"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
-      <c r="B73" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
-      <c r="B74" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C75" s="1"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C76" s="1"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
-      <c r="B77" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C77" s="1"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-    </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="B78" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C78" s="1"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C81" s="1">
-        <v>1</v>
-      </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
+      <c r="B50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="3">
+        <f>SUM(C4:C49)</f>
+        <v>5</v>
+      </c>
+      <c r="D50" s="3">
+        <f>SUM(D4:D49)</f>
+        <v>0</v>
+      </c>
+      <c r="E50" s="3">
+        <f>SUM(E4:E49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="6"/>
-      <c r="B82" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C82" s="1">
-        <v>1</v>
-      </c>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="6"/>
-      <c r="B83" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C83" s="1">
-        <v>1</v>
-      </c>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F83" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="6"/>
-      <c r="B84" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C84" s="1">
-        <v>1</v>
-      </c>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F84" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="6"/>
-      <c r="B85" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C85" s="1">
-        <v>1</v>
-      </c>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="3">
-        <f>SUM(C4:C85)</f>
-        <v>5</v>
-      </c>
-      <c r="D86" s="3">
-        <f>SUM(D4:D85)</f>
-        <v>0</v>
-      </c>
-      <c r="E86" s="3">
-        <f>SUM(E4:E85)</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Coverage for EmailService
</commit_message>
<xml_diff>
--- a/Sprints/Sprint2/G4CapstoneProject_Sprint2_Backlog_Burndown.xlsx
+++ b/Sprints/Sprint2/G4CapstoneProject_Sprint2_Backlog_Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmad\Documents\GitHub\Capstone-Project\Sprints\Sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdena1\source\repos\Capstone-Project\sprints\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BBB147-9A49-42B1-B438-98D7462E1B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B1BFED-105E-491A-8AD9-3FFEDBA6708D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5730" yWindow="2550" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22920" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t>Related User Story</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>Trindiad</t>
-  </si>
-  <si>
-    <t>Nick/Ahmad</t>
   </si>
 </sst>
 </file>
@@ -263,7 +260,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -271,40 +268,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +457,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>45.5</c:v>
+                  <c:v>60.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.5</c:v>
@@ -1470,731 +1507,809 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="14" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="5" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="12">
         <v>4</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="16">
         <v>3</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="16">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="12">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D5" s="16">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="12">
         <v>2</v>
       </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D6" s="16">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="12">
         <v>2</v>
       </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="D7" s="16">
+        <v>1</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="12">
         <v>2</v>
       </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16">
+        <v>0</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="12">
         <v>2</v>
       </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="1" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="12">
         <v>2</v>
       </c>
-      <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="D10" s="16">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="12">
         <v>4</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="16">
         <v>3</v>
       </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" s="16">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="12">
         <v>2</v>
       </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="1" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="12">
         <v>2</v>
       </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="D13" s="16">
+        <v>1</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="1" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="12">
         <v>2</v>
       </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="D14" s="16">
+        <v>1</v>
+      </c>
+      <c r="E14" s="16">
+        <v>0</v>
+      </c>
+      <c r="F14" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="1" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="12">
         <v>2</v>
       </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="12">
         <v>2</v>
       </c>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="D16" s="16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="1" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="12">
         <v>2</v>
       </c>
-      <c r="D17" s="2">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="D17" s="16">
+        <v>1</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="C18" s="12">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0</v>
+      </c>
+      <c r="F18" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="12">
         <v>2</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" t="s">
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="1" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" t="s">
+      <c r="C21" s="12"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" t="s">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="12">
         <v>2</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" t="s">
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="1" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" t="s">
+      <c r="C24" s="12"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="12">
         <v>2</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" t="s">
+      <c r="D26" s="16">
+        <v>0</v>
+      </c>
+      <c r="E26" s="16">
+        <v>0</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="12">
+        <v>2</v>
+      </c>
+      <c r="D27" s="16">
+        <v>0</v>
+      </c>
+      <c r="E27" s="16">
+        <v>0</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="12">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16">
+        <v>0</v>
+      </c>
+      <c r="E28" s="16">
+        <v>0</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="12">
+        <v>2</v>
+      </c>
+      <c r="D29" s="16">
+        <v>0</v>
+      </c>
+      <c r="E29" s="16">
+        <v>0</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="F30" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="12">
+        <v>2</v>
+      </c>
+      <c r="D32" s="16">
+        <v>0</v>
+      </c>
+      <c r="E32" s="16">
+        <v>0</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="12">
+        <v>2</v>
+      </c>
+      <c r="D33" s="16">
+        <v>0</v>
+      </c>
+      <c r="E33" s="16">
+        <v>0</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="12">
+        <v>2</v>
+      </c>
+      <c r="D34" s="16">
+        <v>0</v>
+      </c>
+      <c r="E34" s="16">
+        <v>0</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="E36" s="16">
+        <v>0</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="12">
+        <v>2</v>
+      </c>
+      <c r="D38" s="16">
+        <v>0</v>
+      </c>
+      <c r="E38" s="16">
+        <v>0</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="12">
+        <v>2</v>
+      </c>
+      <c r="D39" s="16">
+        <v>0</v>
+      </c>
+      <c r="E39" s="16">
+        <v>0</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="12">
+        <v>1</v>
+      </c>
+      <c r="D43" s="16">
+        <v>1</v>
+      </c>
+      <c r="E43" s="16"/>
+      <c r="F43" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="12">
+        <v>1</v>
+      </c>
+      <c r="D44" s="16">
+        <v>1</v>
+      </c>
+      <c r="E44" s="16">
+        <v>0</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="12">
+        <v>1</v>
+      </c>
+      <c r="D45" s="16">
+        <v>1</v>
+      </c>
+      <c r="E45" s="16">
+        <v>0</v>
+      </c>
+      <c r="F45" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="12">
+        <v>1</v>
+      </c>
+      <c r="D46" s="16">
+        <v>1</v>
+      </c>
+      <c r="E46" s="16">
+        <v>0</v>
+      </c>
+      <c r="F46" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D36" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2">
-        <v>1</v>
-      </c>
-      <c r="E43" s="2"/>
-      <c r="F43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2">
-        <v>1</v>
-      </c>
-      <c r="E44" s="2"/>
-      <c r="F44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2">
-        <v>1</v>
-      </c>
-      <c r="E45" s="2">
-        <v>0</v>
-      </c>
-      <c r="F45" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-      <c r="D46" s="2">
-        <v>1</v>
-      </c>
-      <c r="E46" s="2">
-        <v>0</v>
-      </c>
-      <c r="F46" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="1" t="s">
+      <c r="A47" s="7"/>
+      <c r="B47" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1</v>
-      </c>
-      <c r="E47" s="2"/>
-      <c r="F47" t="s">
+      <c r="C47" s="12">
+        <v>1</v>
+      </c>
+      <c r="D47" s="16">
+        <v>1</v>
+      </c>
+      <c r="E47" s="16">
+        <v>0</v>
+      </c>
+      <c r="F47" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="13">
         <f>SUM(C4:C47)</f>
-        <v>45.5</v>
-      </c>
-      <c r="D48" s="3">
+        <v>60.5</v>
+      </c>
+      <c r="D48" s="13">
         <f>SUM(D4:D47)</f>
         <v>25.5</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="13">
         <f>SUM(E4:E47)</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F79" t="s">
+      <c r="F79" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="80" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F80" t="s">
+      <c r="F80" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="81" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F81" t="s">
+      <c r="F81" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="82" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F82" t="s">
+      <c r="F82" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="83" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F83" t="s">
+      <c r="F83" s="14" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>